<commit_message>
updates soil multifunctionality code
</commit_message>
<xml_diff>
--- a/Meta_analysis/Metaanalysis_dataset.xlsx
+++ b/Meta_analysis/Metaanalysis_dataset.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amara\Desktop\PhDcode\Meta_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F41150A-21EB-4248-B05A-0E5126C514FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CBF895-A386-42C9-A4D5-5AE0677F806A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="WOS_download1" sheetId="1" r:id="rId1"/>
     <sheet name="my_datasheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">my_datasheet!$A$1:$AF$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WOS_download1!$A$1:$Y$576</definedName>
     <definedName name="ExternalData_1" localSheetId="0">WOS_download1!$B$1:$J$574</definedName>
   </definedNames>
@@ -46,7 +47,7 @@
     <author>Amara</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{D84F99D3-E6AD-4EFE-A6A4-FCA0AC0201C1}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{D84F99D3-E6AD-4EFE-A6A4-FCA0AC0201C1}">
       <text>
         <r>
           <rPr>
@@ -75,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6844" uniqueCount="2959">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7116" uniqueCount="3032">
   <si>
     <t>AUTHORS</t>
   </si>
@@ -8717,9 +8718,6 @@
     <t>Other_disturbances</t>
   </si>
   <si>
-    <t>Control</t>
-  </si>
-  <si>
     <t>Method_ECM_measurement</t>
   </si>
   <si>
@@ -8894,9 +8892,6 @@
     <t>Sampling_year</t>
   </si>
   <si>
-    <t>Northern_Canada</t>
-  </si>
-  <si>
     <t>ITS2</t>
   </si>
   <si>
@@ -8952,17 +8947,249 @@
   </si>
   <si>
     <t>Both descriptive study and bioassay</t>
+  </si>
+  <si>
+    <t>Not much information about the fire. Probably will be discarded</t>
+  </si>
+  <si>
+    <t>Tasmania</t>
+  </si>
+  <si>
+    <t>Eucalyptus</t>
+  </si>
+  <si>
+    <t>Sporocarp_survey</t>
+  </si>
+  <si>
+    <t>Sporocarps</t>
+  </si>
+  <si>
+    <t>2017; 2018; 2019</t>
+  </si>
+  <si>
+    <t>Great_Smoky_Mt</t>
+  </si>
+  <si>
+    <t>Prefire</t>
+  </si>
+  <si>
+    <t>Quercus_suber</t>
+  </si>
+  <si>
+    <t>Root_colonization; DNA</t>
+  </si>
+  <si>
+    <t>PCR?</t>
+  </si>
+  <si>
+    <t>Northwest_Territories</t>
+  </si>
+  <si>
+    <t>Northwest_Territories; Yukon</t>
+  </si>
+  <si>
+    <t>2.85Mha</t>
+  </si>
+  <si>
+    <t>Picea_mariana</t>
+  </si>
+  <si>
+    <t>Prefire; Unburnt</t>
+  </si>
+  <si>
+    <t>Culture</t>
+  </si>
+  <si>
+    <t>Eucalyptus_diversicolor</t>
+  </si>
+  <si>
+    <t>N_burned sites</t>
+  </si>
+  <si>
+    <t>1998; 2002</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Boreal</t>
+  </si>
+  <si>
+    <t>Pinus_sylvestris</t>
+  </si>
+  <si>
+    <t>RFLP</t>
+  </si>
+  <si>
+    <t>Quercus_garryana</t>
+  </si>
+  <si>
+    <t>Control_type</t>
+  </si>
+  <si>
+    <t>N_total_sites</t>
+  </si>
+  <si>
+    <t>N_total_samples</t>
+  </si>
+  <si>
+    <t>No control. No replications</t>
+  </si>
+  <si>
+    <t>Does not approach wildfires as a treatment</t>
+  </si>
+  <si>
+    <t>Management (clearing and grazing)</t>
+  </si>
+  <si>
+    <t>0-5</t>
+  </si>
+  <si>
+    <t>rRNA</t>
+  </si>
+  <si>
+    <t>16S; 18S</t>
+  </si>
+  <si>
+    <t>Southeastern_Australia</t>
+  </si>
+  <si>
+    <t>Semiarid</t>
+  </si>
+  <si>
+    <t>Northeastern_Australia</t>
+  </si>
+  <si>
+    <t>1995; 1996</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Pyrosequencing</t>
+  </si>
+  <si>
+    <t>Caution!! They talk about fungal communities in general, not just ECM</t>
+  </si>
+  <si>
+    <t>Prescribed_fire</t>
+  </si>
+  <si>
+    <t>1; 2</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Need to find the database. They don't provide raw data. Methods are very scarce</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
+  <si>
+    <t>Sclerotia</t>
+  </si>
+  <si>
+    <t>Sampling design layout unclear</t>
+  </si>
+  <si>
+    <t>&lt;1</t>
+  </si>
+  <si>
+    <t>None of the treatments approaches our question. The ones that are burned are agricultural fields, and forest have been undisturbed for more than 60 years</t>
+  </si>
+  <si>
+    <t>Sampling design does not meet the necessary criteria</t>
+  </si>
+  <si>
+    <t>Descriptive; field_experiment</t>
+  </si>
+  <si>
+    <t>Cistus_ladanifer</t>
+  </si>
+  <si>
+    <t>0-20</t>
+  </si>
+  <si>
+    <t>Guild_studied</t>
+  </si>
+  <si>
+    <t>The article is focused on other topic so results about fungal community in burned vs unburned soil is not sufficient</t>
+  </si>
+  <si>
+    <t>Is a discussion article</t>
+  </si>
+  <si>
+    <t>Sites afected by wildfires are more than 30 y-old. Only one stand burned 15 years ago</t>
+  </si>
+  <si>
+    <t>Focused in boletis edulis ONLY. Probably will be discarded. Also only one site but many sampling plots.</t>
+  </si>
+  <si>
+    <t>Boletus_edulis</t>
+  </si>
+  <si>
+    <t>2013; 2014</t>
+  </si>
+  <si>
+    <t>Clearing</t>
+  </si>
+  <si>
+    <t>0-26</t>
+  </si>
+  <si>
+    <t>Perfect</t>
+  </si>
+  <si>
+    <t>Eastern_Australia</t>
+  </si>
+  <si>
+    <t>NO replication. Only one site per fire intensity and 3 plots per site</t>
+  </si>
+  <si>
+    <t>Tropical</t>
+  </si>
+  <si>
+    <t>Hypogeous</t>
+  </si>
+  <si>
+    <t>Allocasuarina</t>
+  </si>
+  <si>
+    <t>Low-medium</t>
+  </si>
+  <si>
+    <t>&gt;1000</t>
+  </si>
+  <si>
+    <t>Only 1 UB site. Samples from potoro feces (only hypogeous fungi)</t>
+  </si>
+  <si>
+    <t>No replication. Only 1 site per treatment in each natural reserve</t>
+  </si>
+  <si>
+    <t>No replicates of each fire…</t>
+  </si>
+  <si>
+    <t>Last fire event in 1970 (more than 45 years ago)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -9025,7 +9252,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -9080,6 +9307,72 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFD9F2D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFD9F2D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor rgb="FFD9F2D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor rgb="FFD9F2D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor rgb="FFD9F2D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor rgb="FFD9F2D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FFD9F2D0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -9099,33 +9392,49 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -9345,8 +9654,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B390" sqref="B390"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R584" sqref="R583:R584"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -9360,14 +9669,14 @@
     <col min="9" max="9" width="5.26953125" customWidth="1"/>
     <col min="10" max="10" width="80.7265625" customWidth="1"/>
     <col min="11" max="11" width="13.08984375" customWidth="1"/>
-    <col min="12" max="12" width="8.6328125" customWidth="1"/>
+    <col min="12" max="12" width="18.26953125" customWidth="1"/>
     <col min="13" max="13" width="12.36328125" customWidth="1"/>
     <col min="14" max="25" width="8.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>2917</v>
+        <v>2916</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -9400,7 +9709,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>2904</v>
+        <v>2903</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>10</v>
@@ -9412,13 +9721,13 @@
         <v>12</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>2895</v>
+        <v>2894</v>
       </c>
       <c r="Q1" s="17" t="s">
-        <v>2903</v>
+        <v>2902</v>
       </c>
       <c r="R1" s="17" t="s">
-        <v>2905</v>
+        <v>2904</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -9472,7 +9781,7 @@
         <v>22</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>2915</v>
+        <v>2914</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -9526,7 +9835,7 @@
         <v>20</v>
       </c>
       <c r="R3" s="18" t="s">
-        <v>2925</v>
+        <v>2924</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -9628,7 +9937,7 @@
         <v>20</v>
       </c>
       <c r="R5" s="18" t="s">
-        <v>2906</v>
+        <v>2905</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -9825,7 +10134,7 @@
       </c>
       <c r="P9" s="7"/>
       <c r="Q9" s="5" t="s">
-        <v>2916</v>
+        <v>2915</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -9879,7 +10188,7 @@
         <v>20</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>2918</v>
+        <v>2917</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -9927,6 +10236,9 @@
         <v>23</v>
       </c>
       <c r="P11" s="7"/>
+      <c r="Q11" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
@@ -9973,6 +10285,9 @@
         <v>23</v>
       </c>
       <c r="P12" s="5"/>
+      <c r="Q12" s="5" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
@@ -10119,7 +10434,7 @@
         <v>20</v>
       </c>
       <c r="R15" s="7" t="s">
-        <v>2924</v>
+        <v>2923</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -10170,7 +10485,7 @@
       </c>
       <c r="P16" s="5"/>
     </row>
-    <row r="17" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -10218,7 +10533,7 @@
       </c>
       <c r="P17" s="7"/>
     </row>
-    <row r="18" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -10264,7 +10579,7 @@
       </c>
       <c r="P18" s="5"/>
     </row>
-    <row r="19" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -10307,10 +10622,10 @@
         <v>36</v>
       </c>
       <c r="P19" s="7" t="s">
-        <v>2885</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2884</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -10358,7 +10673,7 @@
       </c>
       <c r="P20" s="5"/>
     </row>
-    <row r="21" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -10404,7 +10719,7 @@
       </c>
       <c r="P21" s="7"/>
     </row>
-    <row r="22" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -10450,7 +10765,7 @@
       </c>
       <c r="P22" s="5"/>
     </row>
-    <row r="23" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -10498,7 +10813,7 @@
       </c>
       <c r="P23" s="7"/>
     </row>
-    <row r="24" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -10546,7 +10861,7 @@
       </c>
       <c r="P24" s="5"/>
     </row>
-    <row r="25" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -10594,7 +10909,7 @@
       </c>
       <c r="P25" s="7"/>
     </row>
-    <row r="26" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -10640,7 +10955,7 @@
       </c>
       <c r="P26" s="5"/>
     </row>
-    <row r="27" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -10688,7 +11003,7 @@
       </c>
       <c r="P27" s="7"/>
     </row>
-    <row r="28" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -10734,7 +11049,7 @@
       </c>
       <c r="P28" s="5"/>
     </row>
-    <row r="29" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -10782,7 +11097,7 @@
       </c>
       <c r="P29" s="7"/>
     </row>
-    <row r="30" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -10827,8 +11142,11 @@
         <v>23</v>
       </c>
       <c r="P30" s="5"/>
-    </row>
-    <row r="31" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q30" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -10874,7 +11192,7 @@
       </c>
       <c r="P31" s="7"/>
     </row>
-    <row r="32" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -11429,7 +11747,7 @@
         <v>269</v>
       </c>
       <c r="P43" s="7" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -12555,7 +12873,7 @@
         <v>269</v>
       </c>
       <c r="P67" s="7" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="68" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -13498,7 +13816,7 @@
         <v>36</v>
       </c>
       <c r="O87" s="7" t="s">
-        <v>2887</v>
+        <v>2886</v>
       </c>
       <c r="P87" s="7"/>
     </row>
@@ -16944,7 +17262,7 @@
       </c>
       <c r="P160" s="5"/>
     </row>
-    <row r="161" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -16992,7 +17310,7 @@
       </c>
       <c r="P161" s="7"/>
     </row>
-    <row r="162" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -17038,7 +17356,7 @@
       </c>
       <c r="P162" s="5"/>
     </row>
-    <row r="163" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -17086,7 +17404,7 @@
       </c>
       <c r="P163" s="7"/>
     </row>
-    <row r="164" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -17132,7 +17450,7 @@
       </c>
       <c r="P164" s="5"/>
     </row>
-    <row r="165" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -17180,7 +17498,7 @@
       </c>
       <c r="P165" s="7"/>
     </row>
-    <row r="166" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -17228,7 +17546,7 @@
       </c>
       <c r="P166" s="5"/>
     </row>
-    <row r="167" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -17274,7 +17592,7 @@
       </c>
       <c r="P167" s="7"/>
     </row>
-    <row r="168" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -17322,7 +17640,7 @@
       </c>
       <c r="P168" s="5"/>
     </row>
-    <row r="169" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -17368,7 +17686,7 @@
       </c>
       <c r="P169" s="7"/>
     </row>
-    <row r="170" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -17416,7 +17734,7 @@
       </c>
       <c r="P170" s="5"/>
     </row>
-    <row r="171" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -17461,8 +17779,11 @@
         <v>23</v>
       </c>
       <c r="P171" s="7"/>
-    </row>
-    <row r="172" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q171" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="172" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -17510,7 +17831,7 @@
       </c>
       <c r="P172" s="5"/>
     </row>
-    <row r="173" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -17558,7 +17879,7 @@
       </c>
       <c r="P173" s="7"/>
     </row>
-    <row r="174" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -17606,7 +17927,7 @@
       </c>
       <c r="P174" s="5"/>
     </row>
-    <row r="175" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -17652,7 +17973,7 @@
       </c>
       <c r="P175" s="7"/>
     </row>
-    <row r="176" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -17700,7 +18021,7 @@
       </c>
       <c r="P176" s="5"/>
     </row>
-    <row r="177" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -17748,7 +18069,7 @@
       </c>
       <c r="P177" s="7"/>
     </row>
-    <row r="178" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -17796,7 +18117,7 @@
       </c>
       <c r="P178" s="5"/>
     </row>
-    <row r="179" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -17842,7 +18163,7 @@
       </c>
       <c r="P179" s="7"/>
     </row>
-    <row r="180" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -17888,7 +18209,7 @@
       </c>
       <c r="P180" s="5"/>
     </row>
-    <row r="181" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -17934,7 +18255,7 @@
       </c>
       <c r="P181" s="7"/>
     </row>
-    <row r="182" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -17982,7 +18303,7 @@
       </c>
       <c r="P182" s="5"/>
     </row>
-    <row r="183" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -18028,7 +18349,7 @@
       </c>
       <c r="P183" s="7"/>
     </row>
-    <row r="184" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -18074,7 +18395,7 @@
       </c>
       <c r="P184" s="5"/>
     </row>
-    <row r="185" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -18122,7 +18443,7 @@
       </c>
       <c r="P185" s="7"/>
     </row>
-    <row r="186" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -18170,7 +18491,7 @@
       </c>
       <c r="P186" s="5"/>
     </row>
-    <row r="187" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -18216,7 +18537,7 @@
       </c>
       <c r="P187" s="7"/>
     </row>
-    <row r="188" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -18263,10 +18584,10 @@
         <v>269</v>
       </c>
       <c r="P188" s="7" t="s">
-        <v>2886</v>
-      </c>
-    </row>
-    <row r="189" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2885</v>
+      </c>
+    </row>
+    <row r="189" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -18311,8 +18632,11 @@
         <v>23</v>
       </c>
       <c r="P189" s="7"/>
-    </row>
-    <row r="190" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q189" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="190" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -18360,7 +18684,7 @@
       </c>
       <c r="P190" s="5"/>
     </row>
-    <row r="191" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -18406,7 +18730,7 @@
       </c>
       <c r="P191" s="7"/>
     </row>
-    <row r="192" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -18589,7 +18913,7 @@
         <v>1106</v>
       </c>
       <c r="P195" s="7" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="196" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -19761,7 +20085,7 @@
         <v>23</v>
       </c>
       <c r="P220" s="4" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="221" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -20327,7 +20651,7 @@
         <v>1106</v>
       </c>
       <c r="P232" s="14" t="s">
-        <v>2893</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="233" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -20513,7 +20837,7 @@
         <v>23</v>
       </c>
       <c r="P236" s="4" t="s">
-        <v>2927</v>
+        <v>2926</v>
       </c>
     </row>
     <row r="237" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -21163,14 +21487,14 @@
         <v>22</v>
       </c>
       <c r="L250" s="4"/>
-      <c r="M250" s="4" t="s">
-        <v>22</v>
+      <c r="M250" s="14" t="s">
+        <v>268</v>
       </c>
       <c r="N250" s="5" t="s">
         <v>22</v>
       </c>
       <c r="O250" s="5" t="s">
-        <v>23</v>
+        <v>269</v>
       </c>
       <c r="P250" s="4"/>
     </row>
@@ -21917,7 +22241,7 @@
         <v>36</v>
       </c>
       <c r="P266" s="14" t="s">
-        <v>2888</v>
+        <v>2887</v>
       </c>
     </row>
     <row r="267" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -23605,7 +23929,7 @@
         <v>23</v>
       </c>
       <c r="P302" s="22" t="s">
-        <v>2889</v>
+        <v>2888</v>
       </c>
     </row>
     <row r="303" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -24449,7 +24773,7 @@
         <v>23</v>
       </c>
       <c r="P320" s="14" t="s">
-        <v>2890</v>
+        <v>2889</v>
       </c>
     </row>
     <row r="321" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -24637,7 +24961,7 @@
         <v>36</v>
       </c>
       <c r="P324" s="14" t="s">
-        <v>2885</v>
+        <v>2884</v>
       </c>
     </row>
     <row r="325" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -25107,7 +25431,7 @@
         <v>23</v>
       </c>
       <c r="P334" s="4" t="s">
-        <v>2926</v>
+        <v>2925</v>
       </c>
     </row>
     <row r="335" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -25959,7 +26283,7 @@
         <v>36</v>
       </c>
       <c r="P352" s="14" t="s">
-        <v>2891</v>
+        <v>2890</v>
       </c>
     </row>
     <row r="353" spans="1:25" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -26199,6 +26523,9 @@
         <v>23</v>
       </c>
       <c r="P357" s="6"/>
+      <c r="Q357" s="13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="358" spans="1:25" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A358" s="1">
@@ -26628,7 +26955,7 @@
       </c>
       <c r="P366" s="4"/>
     </row>
-    <row r="367" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:25" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A367" s="1">
         <v>366</v>
       </c>
@@ -26673,6 +27000,12 @@
         <v>23</v>
       </c>
       <c r="P367" s="6"/>
+      <c r="Q367" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="R367" s="13" t="s">
+        <v>2957</v>
+      </c>
     </row>
     <row r="368" spans="1:25" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A368" s="8">
@@ -26721,7 +27054,7 @@
         <v>269</v>
       </c>
       <c r="P368" s="9" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
       <c r="Q368" s="8"/>
       <c r="R368" s="8"/>
@@ -27384,7 +27717,7 @@
         <v>1256</v>
       </c>
       <c r="P382" s="7" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="383" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -27768,7 +28101,7 @@
         <v>22</v>
       </c>
       <c r="R390" s="14" t="s">
-        <v>2958</v>
+        <v>2956</v>
       </c>
     </row>
     <row r="391" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -28100,7 +28433,7 @@
         <v>22</v>
       </c>
       <c r="R397" s="13" t="s">
-        <v>2950</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="398" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -28896,7 +29229,7 @@
         <v>269</v>
       </c>
       <c r="P414" s="14" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="415" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -29176,7 +29509,7 @@
         <v>23</v>
       </c>
       <c r="P420" s="14" t="s">
-        <v>2946</v>
+        <v>2944</v>
       </c>
     </row>
     <row r="421" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -29320,7 +29653,7 @@
         <v>269</v>
       </c>
       <c r="P423" s="13" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="424" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -29648,7 +29981,7 @@
         <v>269</v>
       </c>
       <c r="P430" s="14" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="431" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -30168,7 +30501,7 @@
         <v>2261</v>
       </c>
       <c r="P441" s="13" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="442" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -30214,7 +30547,7 @@
         <v>1256</v>
       </c>
       <c r="P442" s="7" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="443" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -30732,7 +31065,7 @@
         <v>22</v>
       </c>
       <c r="R453" s="13" t="s">
-        <v>2941</v>
+        <v>2939</v>
       </c>
     </row>
     <row r="454" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -30778,7 +31111,7 @@
         <v>1608</v>
       </c>
       <c r="P454" s="7" t="s">
-        <v>2892</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="455" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -31394,7 +31727,7 @@
         <v>269</v>
       </c>
       <c r="P467" s="13" t="s">
-        <v>2886</v>
+        <v>2885</v>
       </c>
     </row>
     <row r="468" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -32092,7 +32425,7 @@
         <v>22</v>
       </c>
       <c r="R482" s="14" t="s">
-        <v>2937</v>
+        <v>2936</v>
       </c>
     </row>
     <row r="483" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -32277,7 +32610,7 @@
       </c>
       <c r="P486" s="4"/>
     </row>
-    <row r="487" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:18" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A487" s="1">
         <v>486</v>
       </c>
@@ -32320,6 +32653,12 @@
         <v>23</v>
       </c>
       <c r="P487" s="6"/>
+      <c r="Q487" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="R487" s="39" t="s">
+        <v>3031</v>
+      </c>
     </row>
     <row r="488" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A488" s="1">
@@ -32412,6 +32751,12 @@
         <v>23</v>
       </c>
       <c r="P489" s="6"/>
+      <c r="Q489" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="R489" s="39" t="s">
+        <v>3030</v>
+      </c>
     </row>
     <row r="490" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A490" s="1">
@@ -32506,6 +32851,12 @@
         <v>23</v>
       </c>
       <c r="P491" s="6"/>
+      <c r="Q491" s="39" t="s">
+        <v>20</v>
+      </c>
+      <c r="R491" s="39" t="s">
+        <v>3029</v>
+      </c>
     </row>
     <row r="492" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A492" s="1">
@@ -32552,6 +32903,9 @@
         <v>23</v>
       </c>
       <c r="P492" s="4"/>
+      <c r="Q492" s="37" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="493" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A493" s="1">
@@ -32646,6 +33000,12 @@
         <v>23</v>
       </c>
       <c r="P494" s="4"/>
+      <c r="Q494" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="R494" s="37" t="s">
+        <v>3022</v>
+      </c>
     </row>
     <row r="495" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A495" s="1">
@@ -32741,7 +33101,7 @@
       </c>
       <c r="P496" s="4"/>
     </row>
-    <row r="497" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="497" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A497" s="1">
         <v>496</v>
       </c>
@@ -32788,10 +33148,10 @@
         <v>2261</v>
       </c>
       <c r="P497" s="13" t="s">
-        <v>2886</v>
-      </c>
-    </row>
-    <row r="498" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2885</v>
+      </c>
+    </row>
+    <row r="498" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A498" s="1">
         <v>497</v>
       </c>
@@ -32836,8 +33196,14 @@
         <v>23</v>
       </c>
       <c r="P498" s="4"/>
-    </row>
-    <row r="499" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q498" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="R498" s="14" t="s">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="499" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A499" s="1">
         <v>498</v>
       </c>
@@ -32882,8 +33248,14 @@
         <v>23</v>
       </c>
       <c r="P499" s="6"/>
-    </row>
-    <row r="500" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q499" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="R499" s="13" t="s">
+        <v>3015</v>
+      </c>
+    </row>
+    <row r="500" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A500" s="1">
         <v>499</v>
       </c>
@@ -32931,7 +33303,7 @@
       </c>
       <c r="P500" s="4"/>
     </row>
-    <row r="501" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="501" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A501" s="1">
         <v>500</v>
       </c>
@@ -32974,10 +33346,10 @@
         <v>2215</v>
       </c>
       <c r="P501" s="14" t="s">
-        <v>2894</v>
-      </c>
-    </row>
-    <row r="502" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2893</v>
+      </c>
+    </row>
+    <row r="502" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A502" s="1">
         <v>501</v>
       </c>
@@ -33025,7 +33397,7 @@
       </c>
       <c r="P502" s="4"/>
     </row>
-    <row r="503" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="503" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A503" s="1">
         <v>502</v>
       </c>
@@ -33067,9 +33439,14 @@
       <c r="O503" s="7" t="s">
         <v>2215</v>
       </c>
-      <c r="P503" s="6"/>
-    </row>
-    <row r="504" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P503" s="13" t="s">
+        <v>1431</v>
+      </c>
+      <c r="Q503" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="504" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A504" s="1">
         <v>503</v>
       </c>
@@ -33117,7 +33494,7 @@
       </c>
       <c r="P504" s="4"/>
     </row>
-    <row r="505" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="505" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A505" s="1">
         <v>504</v>
       </c>
@@ -33165,7 +33542,7 @@
       </c>
       <c r="P505" s="6"/>
     </row>
-    <row r="506" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="506" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A506" s="1">
         <v>505</v>
       </c>
@@ -33213,7 +33590,7 @@
       </c>
       <c r="P506" s="4"/>
     </row>
-    <row r="507" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="507" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A507" s="1">
         <v>506</v>
       </c>
@@ -33259,7 +33636,7 @@
       </c>
       <c r="P507" s="6"/>
     </row>
-    <row r="508" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="508" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A508" s="1">
         <v>507</v>
       </c>
@@ -33307,7 +33684,7 @@
       </c>
       <c r="P508" s="4"/>
     </row>
-    <row r="509" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="509" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A509" s="1">
         <v>508</v>
       </c>
@@ -33350,8 +33727,12 @@
         <v>23</v>
       </c>
       <c r="P509" s="6"/>
-    </row>
-    <row r="510" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q509" s="13"/>
+      <c r="R509" s="13" t="s">
+        <v>3014</v>
+      </c>
+    </row>
+    <row r="510" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A510" s="1">
         <v>509</v>
       </c>
@@ -33399,7 +33780,7 @@
       </c>
       <c r="P510" s="4"/>
     </row>
-    <row r="511" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="511" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A511" s="1">
         <v>510</v>
       </c>
@@ -33445,7 +33826,7 @@
       </c>
       <c r="P511" s="6"/>
     </row>
-    <row r="512" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="512" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A512" s="1">
         <v>511</v>
       </c>
@@ -33493,7 +33874,7 @@
       </c>
       <c r="P512" s="4"/>
     </row>
-    <row r="513" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="513" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A513" s="1">
         <v>512</v>
       </c>
@@ -33541,7 +33922,7 @@
       </c>
       <c r="P513" s="6"/>
     </row>
-    <row r="514" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="514" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A514" s="1">
         <v>513</v>
       </c>
@@ -33589,7 +33970,7 @@
       </c>
       <c r="P514" s="4"/>
     </row>
-    <row r="515" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="515" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A515" s="1">
         <v>514</v>
       </c>
@@ -33635,7 +34016,7 @@
       </c>
       <c r="P515" s="6"/>
     </row>
-    <row r="516" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="516" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A516" s="1">
         <v>515</v>
       </c>
@@ -33683,7 +34064,7 @@
       </c>
       <c r="P516" s="4"/>
     </row>
-    <row r="517" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="517" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A517" s="1">
         <v>516</v>
       </c>
@@ -33731,7 +34112,7 @@
       </c>
       <c r="P517" s="6"/>
     </row>
-    <row r="518" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="518" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A518" s="1">
         <v>517</v>
       </c>
@@ -33777,7 +34158,7 @@
       </c>
       <c r="P518" s="4"/>
     </row>
-    <row r="519" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="519" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A519" s="1">
         <v>518</v>
       </c>
@@ -33825,7 +34206,7 @@
       </c>
       <c r="P519" s="6"/>
     </row>
-    <row r="520" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="520" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A520" s="1">
         <v>519</v>
       </c>
@@ -33870,8 +34251,14 @@
         <v>23</v>
       </c>
       <c r="P520" s="4"/>
-    </row>
-    <row r="521" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q520" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R520" s="14" t="s">
+        <v>3013</v>
+      </c>
+    </row>
+    <row r="521" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A521" s="1">
         <v>520</v>
       </c>
@@ -33916,8 +34303,14 @@
         <v>23</v>
       </c>
       <c r="P521" s="6"/>
-    </row>
-    <row r="522" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q521" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="R521" s="13" t="s">
+        <v>3012</v>
+      </c>
+    </row>
+    <row r="522" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A522" s="1">
         <v>521</v>
       </c>
@@ -33962,8 +34355,11 @@
         <v>23</v>
       </c>
       <c r="P522" s="4"/>
-    </row>
-    <row r="523" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q522" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="523" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A523" s="1">
         <v>522</v>
       </c>
@@ -34011,7 +34407,7 @@
       </c>
       <c r="P523" s="6"/>
     </row>
-    <row r="524" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="524" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A524" s="1">
         <v>523</v>
       </c>
@@ -34057,7 +34453,7 @@
       </c>
       <c r="P524" s="4"/>
     </row>
-    <row r="525" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="525" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A525" s="1">
         <v>524</v>
       </c>
@@ -34102,8 +34498,14 @@
         <v>23</v>
       </c>
       <c r="P525" s="6"/>
-    </row>
-    <row r="526" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q525" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="R525" s="13" t="s">
+        <v>3007</v>
+      </c>
+    </row>
+    <row r="526" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A526" s="1">
         <v>525</v>
       </c>
@@ -34148,8 +34550,14 @@
         <v>23</v>
       </c>
       <c r="P526" s="4"/>
-    </row>
-    <row r="527" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q526" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R526" s="14" t="s">
+        <v>3006</v>
+      </c>
+    </row>
+    <row r="527" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A527" s="1">
         <v>526</v>
       </c>
@@ -34197,7 +34605,7 @@
       </c>
       <c r="P527" s="6"/>
     </row>
-    <row r="528" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="528" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A528" s="1">
         <v>527</v>
       </c>
@@ -34243,7 +34651,7 @@
       </c>
       <c r="P528" s="4"/>
     </row>
-    <row r="529" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="529" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A529" s="1">
         <v>528</v>
       </c>
@@ -34291,7 +34699,7 @@
       </c>
       <c r="P529" s="6"/>
     </row>
-    <row r="530" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="530" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A530" s="1">
         <v>529</v>
       </c>
@@ -34334,10 +34742,10 @@
         <v>36</v>
       </c>
       <c r="P530" s="14" t="s">
-        <v>2885</v>
-      </c>
-    </row>
-    <row r="531" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2884</v>
+      </c>
+    </row>
+    <row r="531" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A531" s="1">
         <v>530</v>
       </c>
@@ -34385,7 +34793,7 @@
       </c>
       <c r="P531" s="6"/>
     </row>
-    <row r="532" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="532" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A532" s="1">
         <v>531</v>
       </c>
@@ -34433,7 +34841,7 @@
       </c>
       <c r="P532" s="4"/>
     </row>
-    <row r="533" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="533" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A533" s="1">
         <v>532</v>
       </c>
@@ -34481,7 +34889,7 @@
       </c>
       <c r="P533" s="6"/>
     </row>
-    <row r="534" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="534" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A534" s="1">
         <v>533</v>
       </c>
@@ -34529,7 +34937,7 @@
       </c>
       <c r="P534" s="4"/>
     </row>
-    <row r="535" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="535" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A535" s="1">
         <v>534</v>
       </c>
@@ -34574,8 +34982,11 @@
         <v>23</v>
       </c>
       <c r="P535" s="6"/>
-    </row>
-    <row r="536" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q535" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="536" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A536" s="1">
         <v>535</v>
       </c>
@@ -34621,7 +35032,7 @@
       </c>
       <c r="P536" s="4"/>
     </row>
-    <row r="537" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="537" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A537" s="1">
         <v>536</v>
       </c>
@@ -34667,7 +35078,7 @@
       </c>
       <c r="P537" s="6"/>
     </row>
-    <row r="538" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="538" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A538" s="1">
         <v>537</v>
       </c>
@@ -34712,8 +35123,14 @@
         <v>23</v>
       </c>
       <c r="P538" s="4"/>
-    </row>
-    <row r="539" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q538" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="R538" s="14" t="s">
+        <v>3004</v>
+      </c>
+    </row>
+    <row r="539" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A539" s="1">
         <v>538</v>
       </c>
@@ -34759,7 +35176,7 @@
       </c>
       <c r="P539" s="6"/>
     </row>
-    <row r="540" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="540" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A540" s="1">
         <v>539</v>
       </c>
@@ -34807,7 +35224,7 @@
       </c>
       <c r="P540" s="4"/>
     </row>
-    <row r="541" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="541" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A541" s="1">
         <v>540</v>
       </c>
@@ -34855,7 +35272,7 @@
       </c>
       <c r="P541" s="6"/>
     </row>
-    <row r="542" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="542" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A542" s="1">
         <v>541</v>
       </c>
@@ -34900,8 +35317,14 @@
         <v>23</v>
       </c>
       <c r="P542" s="4"/>
-    </row>
-    <row r="543" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q542" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="R542" s="14" t="s">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="543" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A543" s="1">
         <v>542</v>
       </c>
@@ -34949,7 +35372,7 @@
       </c>
       <c r="P543" s="6"/>
     </row>
-    <row r="544" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="544" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A544" s="1">
         <v>543</v>
       </c>
@@ -34995,7 +35418,7 @@
       </c>
       <c r="P544" s="4"/>
     </row>
-    <row r="545" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="545" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A545" s="1">
         <v>544</v>
       </c>
@@ -35041,11 +35464,11 @@
       </c>
       <c r="P545" s="6"/>
     </row>
-    <row r="546" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="546" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A546" s="1">
         <v>545</v>
       </c>
-      <c r="B546" s="4" t="s">
+      <c r="B546" s="14" t="s">
         <v>2739</v>
       </c>
       <c r="C546" s="5" t="s">
@@ -35086,8 +35509,11 @@
         <v>23</v>
       </c>
       <c r="P546" s="4"/>
-    </row>
-    <row r="547" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q546" s="14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="547" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A547" s="1">
         <v>546</v>
       </c>
@@ -35131,9 +35557,14 @@
       <c r="O547" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="P547" s="6"/>
-    </row>
-    <row r="548" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P547" s="13" t="s">
+        <v>1431</v>
+      </c>
+      <c r="Q547" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="548" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A548" s="1">
         <v>547</v>
       </c>
@@ -35179,7 +35610,7 @@
       </c>
       <c r="P548" s="4"/>
     </row>
-    <row r="549" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="549" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A549" s="1">
         <v>548</v>
       </c>
@@ -35227,7 +35658,7 @@
       </c>
       <c r="P549" s="6"/>
     </row>
-    <row r="550" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="550" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A550" s="1">
         <v>549</v>
       </c>
@@ -35275,7 +35706,7 @@
       </c>
       <c r="P550" s="4"/>
     </row>
-    <row r="551" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="551" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A551" s="1">
         <v>550</v>
       </c>
@@ -35319,7 +35750,7 @@
       </c>
       <c r="P551" s="6"/>
     </row>
-    <row r="552" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="552" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A552" s="1">
         <v>551</v>
       </c>
@@ -35365,7 +35796,7 @@
       </c>
       <c r="P552" s="4"/>
     </row>
-    <row r="553" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="553" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A553" s="1">
         <v>552</v>
       </c>
@@ -35413,7 +35844,7 @@
       </c>
       <c r="P553" s="6"/>
     </row>
-    <row r="554" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="554" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A554" s="1">
         <v>553</v>
       </c>
@@ -35460,10 +35891,10 @@
         <v>36</v>
       </c>
       <c r="P554" s="14" t="s">
-        <v>2891</v>
-      </c>
-    </row>
-    <row r="555" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+        <v>2890</v>
+      </c>
+    </row>
+    <row r="555" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A555" s="1">
         <v>554</v>
       </c>
@@ -35511,7 +35942,7 @@
       </c>
       <c r="P555" s="6"/>
     </row>
-    <row r="556" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="556" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A556" s="1">
         <v>555</v>
       </c>
@@ -35559,7 +35990,7 @@
       </c>
       <c r="P556" s="4"/>
     </row>
-    <row r="557" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="557" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A557" s="1">
         <v>556</v>
       </c>
@@ -35607,7 +36038,7 @@
       </c>
       <c r="P557" s="6"/>
     </row>
-    <row r="558" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="558" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A558" s="1">
         <v>557</v>
       </c>
@@ -35655,7 +36086,7 @@
       </c>
       <c r="P558" s="4"/>
     </row>
-    <row r="559" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="559" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A559" s="1">
         <v>558</v>
       </c>
@@ -35703,7 +36134,7 @@
       </c>
       <c r="P559" s="6"/>
     </row>
-    <row r="560" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="560" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A560" s="1">
         <v>559</v>
       </c>
@@ -35748,8 +36179,14 @@
         <v>23</v>
       </c>
       <c r="P560" s="4"/>
-    </row>
-    <row r="561" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q560" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="R560" s="14" t="s">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="561" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A561" s="1">
         <v>560</v>
       </c>
@@ -35797,7 +36234,7 @@
       </c>
       <c r="P561" s="6"/>
     </row>
-    <row r="562" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="562" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A562" s="1">
         <v>561</v>
       </c>
@@ -35842,8 +36279,14 @@
         <v>23</v>
       </c>
       <c r="P562" s="4"/>
-    </row>
-    <row r="563" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q562" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="R562" s="38" t="s">
+        <v>3028</v>
+      </c>
+    </row>
+    <row r="563" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A563" s="1">
         <v>562</v>
       </c>
@@ -35888,8 +36331,11 @@
         <v>23</v>
       </c>
       <c r="P563" s="6"/>
-    </row>
-    <row r="564" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q563" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="564" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A564" s="1">
         <v>563</v>
       </c>
@@ -35937,7 +36383,7 @@
       </c>
       <c r="P564" s="4"/>
     </row>
-    <row r="565" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="565" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A565" s="1">
         <v>564</v>
       </c>
@@ -35982,8 +36428,11 @@
         <v>23</v>
       </c>
       <c r="P565" s="6"/>
-    </row>
-    <row r="566" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q565" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="566" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A566" s="1">
         <v>565</v>
       </c>
@@ -36029,7 +36478,7 @@
         <v>1224</v>
       </c>
     </row>
-    <row r="567" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="567" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A567" s="1">
         <v>566</v>
       </c>
@@ -36075,7 +36524,7 @@
       </c>
       <c r="P567" s="6"/>
     </row>
-    <row r="568" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="568" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A568" s="1">
         <v>567</v>
       </c>
@@ -36123,7 +36572,7 @@
       </c>
       <c r="P568" s="4"/>
     </row>
-    <row r="569" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="569" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A569" s="1">
         <v>568</v>
       </c>
@@ -36168,8 +36617,14 @@
         <v>23</v>
       </c>
       <c r="P569" s="6"/>
-    </row>
-    <row r="570" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="Q569" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="R569" s="13" t="s">
+        <v>2986</v>
+      </c>
+    </row>
+    <row r="570" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A570" s="1">
         <v>569</v>
       </c>
@@ -36217,7 +36672,7 @@
       </c>
       <c r="P570" s="4"/>
     </row>
-    <row r="571" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="571" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A571" s="1">
         <v>570</v>
       </c>
@@ -36265,7 +36720,7 @@
       </c>
       <c r="P571" s="6"/>
     </row>
-    <row r="572" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="572" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A572" s="1">
         <v>571</v>
       </c>
@@ -36313,7 +36768,7 @@
       </c>
       <c r="P572" s="4"/>
     </row>
-    <row r="573" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="573" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A573" s="1">
         <v>572</v>
       </c>
@@ -36361,7 +36816,7 @@
       </c>
       <c r="P573" s="6"/>
     </row>
-    <row r="574" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="574" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A574" s="1">
         <v>573</v>
       </c>
@@ -36406,9 +36861,15 @@
         <v>23</v>
       </c>
       <c r="P574" s="11"/>
-    </row>
-    <row r="575" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="576" spans="1:16" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="Q574" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="R574" s="35" t="s">
+        <v>2985</v>
+      </c>
+    </row>
+    <row r="575" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="576" spans="1:18" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="577" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="578" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="579" ht="14.25" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -36837,7 +37298,7 @@
   <autoFilter ref="A1:Y576" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Macrofungal diversity and community ecology in mature and regrowth wet eucalypt forest in Tasmania: A multivariate study"/>
+        <filter val="Communities of tropical soil fungi differ between burned and unburned forest, with corresponding changes in plant community composition, litter and soil chemistry"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -36851,538 +37312,1484 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AB999"/>
+  <dimension ref="A1:AJ1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V16" sqref="V16"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" style="16" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" style="16" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" style="34" customWidth="1"/>
+    <col min="2" max="2" width="9.81640625" style="34" customWidth="1"/>
     <col min="3" max="3" width="11.453125" style="16" customWidth="1"/>
     <col min="4" max="5" width="8.6328125" style="16" customWidth="1"/>
-    <col min="6" max="6" width="10.26953125" style="16" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" style="16" customWidth="1"/>
     <col min="7" max="7" width="8.6328125" style="16" customWidth="1"/>
     <col min="8" max="9" width="11.08984375" style="16" customWidth="1"/>
-    <col min="10" max="11" width="15.90625" style="16" customWidth="1"/>
-    <col min="12" max="12" width="10.08984375" style="16" customWidth="1"/>
-    <col min="13" max="13" width="12.90625" style="16" customWidth="1"/>
-    <col min="14" max="14" width="11.7265625" style="16" customWidth="1"/>
-    <col min="15" max="15" width="13.08984375" style="16" customWidth="1"/>
-    <col min="16" max="16" width="12.36328125" style="16" customWidth="1"/>
-    <col min="17" max="17" width="13.453125" style="16" customWidth="1"/>
-    <col min="18" max="20" width="9" style="16" customWidth="1"/>
-    <col min="21" max="21" width="13" style="16" customWidth="1"/>
-    <col min="22" max="23" width="14.7265625" style="16" customWidth="1"/>
-    <col min="24" max="24" width="14.26953125" style="16" customWidth="1"/>
-    <col min="25" max="25" width="18.90625" style="16" customWidth="1"/>
-    <col min="26" max="26" width="17.453125" style="16" customWidth="1"/>
-    <col min="27" max="41" width="8.6328125" style="16" customWidth="1"/>
-    <col min="42" max="16384" width="12.6328125" style="16"/>
+    <col min="10" max="10" width="13.7265625" style="16" customWidth="1"/>
+    <col min="11" max="12" width="15.90625" style="16" customWidth="1"/>
+    <col min="13" max="13" width="10.08984375" style="16" customWidth="1"/>
+    <col min="14" max="14" width="12.90625" style="16" customWidth="1"/>
+    <col min="15" max="15" width="11.7265625" style="16" customWidth="1"/>
+    <col min="16" max="16" width="13.08984375" style="16" customWidth="1"/>
+    <col min="17" max="17" width="12.36328125" style="16" customWidth="1"/>
+    <col min="18" max="18" width="13.453125" style="16" customWidth="1"/>
+    <col min="19" max="19" width="15.54296875" style="16" customWidth="1"/>
+    <col min="20" max="20" width="13.54296875" style="16" customWidth="1"/>
+    <col min="21" max="21" width="17.1796875" style="16" customWidth="1"/>
+    <col min="22" max="22" width="16.08984375" style="16" customWidth="1"/>
+    <col min="23" max="23" width="15.7265625" style="16" customWidth="1"/>
+    <col min="24" max="24" width="15.81640625" style="16" customWidth="1"/>
+    <col min="25" max="25" width="14.7265625" style="16" customWidth="1"/>
+    <col min="26" max="26" width="13" style="16" customWidth="1"/>
+    <col min="27" max="27" width="14.7265625" style="16" customWidth="1"/>
+    <col min="28" max="28" width="14.26953125" style="16" customWidth="1"/>
+    <col min="29" max="29" width="18.90625" style="16" customWidth="1"/>
+    <col min="30" max="30" width="17.453125" style="16" customWidth="1"/>
+    <col min="31" max="45" width="8.6328125" style="16" customWidth="1"/>
+    <col min="46" max="16384" width="12.6328125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="20" t="s">
-        <v>2917</v>
-      </c>
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:36" s="21" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="25" t="s">
+        <v>2916</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>2870</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="25" t="s">
+        <v>2895</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>2927</v>
+      </c>
+      <c r="E1" s="25" t="s">
+        <v>2937</v>
+      </c>
+      <c r="F1" s="25" t="s">
+        <v>2871</v>
+      </c>
+      <c r="G1" s="25" t="s">
+        <v>2950</v>
+      </c>
+      <c r="H1" s="25" t="s">
+        <v>2872</v>
+      </c>
+      <c r="I1" s="25" t="s">
+        <v>2873</v>
+      </c>
+      <c r="J1" s="32" t="s">
+        <v>3011</v>
+      </c>
+      <c r="K1" s="20" t="s">
         <v>2896</v>
       </c>
-      <c r="D1" s="20" t="s">
-        <v>2928</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>2938</v>
-      </c>
-      <c r="F1" s="20" t="s">
-        <v>2871</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>2952</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>2872</v>
-      </c>
-      <c r="I1" s="20" t="s">
-        <v>2873</v>
-      </c>
-      <c r="J1" s="20" t="s">
+      <c r="L1" s="20" t="s">
         <v>2897</v>
       </c>
-      <c r="K1" s="20" t="s">
-        <v>2898</v>
-      </c>
-      <c r="L1" s="20" t="s">
+      <c r="M1" s="27" t="s">
         <v>2874</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="N1" s="27" t="s">
         <v>2875</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="O1" s="27" t="s">
         <v>2876</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="P1" s="27" t="s">
         <v>2877</v>
       </c>
-      <c r="P1" s="20" t="s">
+      <c r="Q1" s="27" t="s">
         <v>2878</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="R1" s="29" t="s">
         <v>2879</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="S1" s="26" t="s">
+        <v>2982</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>2983</v>
+      </c>
+      <c r="U1" s="28" t="s">
+        <v>2984</v>
+      </c>
+      <c r="V1" s="28" t="s">
+        <v>2930</v>
+      </c>
+      <c r="W1" s="28" t="s">
+        <v>2941</v>
+      </c>
+      <c r="X1" s="28" t="s">
+        <v>2975</v>
+      </c>
+      <c r="Y1" s="28" t="s">
+        <v>2942</v>
+      </c>
+      <c r="Z1" s="30" t="s">
+        <v>2900</v>
+      </c>
+      <c r="AA1" s="30" t="s">
+        <v>2922</v>
+      </c>
+      <c r="AB1" s="31" t="s">
+        <v>2901</v>
+      </c>
+      <c r="AC1" s="32" t="s">
         <v>2880</v>
       </c>
-      <c r="S1" s="20" t="s">
-        <v>2931</v>
-      </c>
-      <c r="T1" s="20" t="s">
-        <v>2943</v>
-      </c>
-      <c r="U1" s="20" t="s">
-        <v>2901</v>
-      </c>
-      <c r="V1" s="20" t="s">
-        <v>2923</v>
-      </c>
-      <c r="W1" s="20" t="s">
-        <v>2944</v>
-      </c>
-      <c r="X1" s="21" t="s">
-        <v>2902</v>
-      </c>
-      <c r="Y1" s="20" t="s">
+      <c r="AD1" s="32" t="s">
         <v>2881</v>
       </c>
-      <c r="Z1" s="20" t="s">
+      <c r="AE1" s="32" t="s">
         <v>2882</v>
       </c>
-      <c r="AA1" s="20" t="s">
+      <c r="AF1" s="33" t="s">
         <v>2883</v>
       </c>
-      <c r="AB1" s="21" t="s">
-        <v>2884</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16">
+      <c r="AG1" s="33"/>
+      <c r="AH1" s="33"/>
+      <c r="AI1" s="33"/>
+      <c r="AJ1" s="33"/>
+    </row>
+    <row r="2" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="34">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="34" t="s">
         <v>13</v>
       </c>
       <c r="D2" s="16">
         <v>2009</v>
       </c>
       <c r="F2" s="16" t="s">
+        <v>2911</v>
+      </c>
+      <c r="K2" s="16" t="s">
         <v>2912</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="L2" s="16" t="s">
         <v>2913</v>
       </c>
-      <c r="K2" s="16" t="s">
-        <v>2914</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="16">
+    </row>
+    <row r="3" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="34">
         <v>5</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="34" t="s">
         <v>44</v>
       </c>
       <c r="D3" s="16">
         <v>2011</v>
       </c>
       <c r="F3" s="16" t="s">
+        <v>2906</v>
+      </c>
+      <c r="H3" s="16" t="s">
         <v>2907</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="I3" s="16" t="s">
         <v>2908</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="K3" s="16" t="s">
         <v>2909</v>
       </c>
-      <c r="J3" s="16" t="s">
+      <c r="M3" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O3" s="16">
+        <v>2004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="34">
+        <v>6</v>
+      </c>
+      <c r="B4" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>2910</v>
-      </c>
-      <c r="L3" s="16" t="s">
-        <v>2900</v>
-      </c>
-      <c r="N3" s="16">
-        <v>2004</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16">
-        <v>6</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>2911</v>
       </c>
       <c r="D4" s="16">
         <v>2023</v>
       </c>
       <c r="F4" s="16" t="s">
-        <v>2907</v>
-      </c>
-      <c r="N4" s="16">
+        <v>2906</v>
+      </c>
+      <c r="O4" s="16">
         <v>2004</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
+    <row r="5" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="34">
         <v>8</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="34" t="s">
         <v>62</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>2899</v>
+        <v>2898</v>
       </c>
       <c r="D5" s="16">
         <v>2007</v>
       </c>
       <c r="F5" s="16" t="s">
+        <v>2911</v>
+      </c>
+      <c r="K5" s="16" t="s">
         <v>2912</v>
       </c>
-      <c r="J5" s="16" t="s">
+      <c r="L5" s="16" t="s">
         <v>2913</v>
       </c>
-      <c r="K5" s="16" t="s">
-        <v>2914</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
+    </row>
+    <row r="6" spans="1:36" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="34">
         <v>10</v>
       </c>
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="34" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="16">
+      <c r="C6" s="23" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D6" s="23">
+        <v>2020</v>
+      </c>
+      <c r="E6" s="23">
+        <v>2015</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>2968</v>
+      </c>
+      <c r="K6" s="23" t="s">
+        <v>2971</v>
+      </c>
+      <c r="M6" s="23" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O6" s="23">
+        <v>2014</v>
+      </c>
+      <c r="P6" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="23" t="s">
+        <v>2970</v>
+      </c>
+      <c r="S6" s="23" t="s">
+        <v>2972</v>
+      </c>
+      <c r="Z6" s="23" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AC6" s="23" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD6" s="23" t="s">
+        <v>2934</v>
+      </c>
+      <c r="AE6" s="23" t="s">
+        <v>2954</v>
+      </c>
+    </row>
+    <row r="7" spans="1:36" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="34">
+        <v>10</v>
+      </c>
+      <c r="B7" s="34" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>2973</v>
+      </c>
+      <c r="D7" s="23">
+        <v>2020</v>
+      </c>
+      <c r="E7" s="23">
+        <v>2015</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>2968</v>
+      </c>
+      <c r="K7" s="23" t="s">
+        <v>2971</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O7" s="23">
+        <v>2014</v>
+      </c>
+      <c r="P7" s="23">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="23" t="s">
+        <v>2970</v>
+      </c>
+      <c r="S7" s="23" t="s">
+        <v>2972</v>
+      </c>
+      <c r="Z7" s="23" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AC7" s="23" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD7" s="23" t="s">
+        <v>2934</v>
+      </c>
+      <c r="AE7" s="23" t="s">
+        <v>2954</v>
+      </c>
+    </row>
+    <row r="8" spans="1:36" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="34">
         <v>11</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B8" s="34" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C8" s="24" t="s">
+        <v>2918</v>
+      </c>
+      <c r="D8" s="24">
+        <v>2010</v>
+      </c>
+      <c r="E8" s="24">
+        <v>2007</v>
+      </c>
+      <c r="F8" s="24" t="s">
         <v>2919</v>
       </c>
-      <c r="D7" s="16">
+      <c r="G8" s="24" t="s">
+        <v>2951</v>
+      </c>
+      <c r="K8" s="24" t="s">
+        <v>2920</v>
+      </c>
+      <c r="L8" s="24" t="s">
+        <v>2965</v>
+      </c>
+      <c r="M8" s="24" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O8" s="24">
+        <v>2003</v>
+      </c>
+      <c r="P8" s="24">
+        <v>4</v>
+      </c>
+      <c r="S8" s="24" t="s">
+        <v>2921</v>
+      </c>
+      <c r="Z8" s="24" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA8" s="24">
+        <v>20</v>
+      </c>
+      <c r="AC8" s="24" t="s">
+        <v>2966</v>
+      </c>
+      <c r="AD8" s="24" t="s">
+        <v>2967</v>
+      </c>
+      <c r="AE8" s="24" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="9" spans="1:36" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="34">
+        <v>11</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" s="24" t="s">
+        <v>2973</v>
+      </c>
+      <c r="D9" s="24">
         <v>2010</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="E9" s="24">
+        <v>2007</v>
+      </c>
+      <c r="F9" s="24" t="s">
+        <v>2919</v>
+      </c>
+      <c r="G9" s="24" t="s">
+        <v>2951</v>
+      </c>
+      <c r="K9" s="24" t="s">
         <v>2920</v>
       </c>
-      <c r="J7" s="16" t="s">
+      <c r="L9" s="24" t="s">
+        <v>2965</v>
+      </c>
+      <c r="M9" s="24" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O9" s="24">
+        <v>2003</v>
+      </c>
+      <c r="P9" s="24">
+        <v>4</v>
+      </c>
+      <c r="S9" s="24" t="s">
         <v>2921</v>
       </c>
-      <c r="L7" s="16" t="s">
-        <v>2900</v>
-      </c>
-      <c r="N7" s="16">
-        <v>2003</v>
-      </c>
-      <c r="O7" s="16">
+      <c r="Z9" s="24" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA9" s="24">
+        <v>20</v>
+      </c>
+      <c r="AC9" s="24" t="s">
+        <v>2966</v>
+      </c>
+      <c r="AD9" s="24" t="s">
+        <v>2967</v>
+      </c>
+      <c r="AE9" s="24" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="10" spans="1:36" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="34">
+        <v>481</v>
+      </c>
+      <c r="B10" s="34" t="s">
+        <v>2449</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D10" s="23">
+        <v>2021</v>
+      </c>
+      <c r="F10" s="23" t="s">
+        <v>2928</v>
+      </c>
+      <c r="K10" s="23" t="s">
+        <v>2929</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>2899</v>
+      </c>
+      <c r="N10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="O10" s="23">
+        <v>2009</v>
+      </c>
+      <c r="P10" s="23">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="R10" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="23" t="s">
+        <v>2921</v>
+      </c>
+      <c r="V10" s="23">
         <v>4</v>
       </c>
-      <c r="R7" s="16" t="s">
-        <v>2922</v>
-      </c>
-      <c r="V7" s="16">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" s="23" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="23">
-        <v>481</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>2449</v>
-      </c>
-      <c r="C8" s="23" t="s">
+      <c r="Z10" s="23" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA10" s="23" t="s">
+        <v>2932</v>
+      </c>
+      <c r="AB10" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC10" s="23" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD10" s="23" t="s">
+        <v>2934</v>
+      </c>
+      <c r="AE10" s="23" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="11" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="34">
+        <v>452</v>
+      </c>
+      <c r="B11" s="34" t="s">
+        <v>2313</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D11" s="16">
+        <v>2022</v>
+      </c>
+      <c r="E11" s="16">
+        <v>2015</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>2969</v>
+      </c>
+      <c r="K11" s="16" t="s">
+        <v>2940</v>
+      </c>
+      <c r="M11" s="16" t="s">
         <v>2899</v>
       </c>
-      <c r="D8" s="23">
+      <c r="O11" s="16">
+        <v>2012</v>
+      </c>
+      <c r="P11" s="16">
+        <v>3</v>
+      </c>
+      <c r="S11" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="W11" s="16">
+        <v>27</v>
+      </c>
+      <c r="Y11" s="16">
+        <v>27</v>
+      </c>
+      <c r="Z11" s="16" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA11" s="16" t="s">
+        <v>2943</v>
+      </c>
+      <c r="AB11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC11" s="16" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD11" s="16" t="s">
+        <v>2934</v>
+      </c>
+      <c r="AE11" s="16" t="s">
+        <v>2938</v>
+      </c>
+    </row>
+    <row r="12" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="34">
+        <v>396</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>2061</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D12" s="16">
+        <v>2004</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>2945</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>2906</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>2940</v>
+      </c>
+      <c r="M12" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O12" s="16">
+        <v>1999</v>
+      </c>
+      <c r="S12" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="Z12" s="16" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA12" s="16" t="s">
+        <v>2946</v>
+      </c>
+      <c r="AB12" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC12" s="16" t="s">
+        <v>2947</v>
+      </c>
+      <c r="AD12" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE12" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:36" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="34">
+        <v>389</v>
+      </c>
+      <c r="B13" s="34" t="s">
+        <v>2028</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D13" s="24">
+        <v>2019</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>2949</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>2951</v>
+      </c>
+      <c r="M13" s="24" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O13" s="24">
+        <v>1995</v>
+      </c>
+      <c r="P13" s="24" t="s">
+        <v>2952</v>
+      </c>
+      <c r="Z13" s="24" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA13" s="24">
+        <v>18</v>
+      </c>
+      <c r="AB13" s="24" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC13" s="24" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD13" s="24" t="s">
+        <v>2953</v>
+      </c>
+      <c r="AE13" s="24" t="s">
+        <v>2954</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" s="24" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="34">
+        <v>389</v>
+      </c>
+      <c r="B14" s="34" t="s">
+        <v>2028</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>2918</v>
+      </c>
+      <c r="D14" s="24">
+        <v>2019</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>2949</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>2951</v>
+      </c>
+      <c r="M14" s="24" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O14" s="24">
+        <v>1995</v>
+      </c>
+      <c r="P14" s="24" t="s">
+        <v>2952</v>
+      </c>
+      <c r="Z14" s="24" t="s">
+        <v>2955</v>
+      </c>
+      <c r="AC14" s="24" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD14" s="24" t="s">
+        <v>2953</v>
+      </c>
+      <c r="AE14" s="24" t="s">
+        <v>2938</v>
+      </c>
+    </row>
+    <row r="15" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="34">
+        <v>366</v>
+      </c>
+      <c r="B15" s="34" t="s">
+        <v>1925</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D15" s="16">
+        <v>2002</v>
+      </c>
+      <c r="E15" s="16">
+        <v>1994</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>2958</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>2959</v>
+      </c>
+      <c r="M15" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="Z15" s="16" t="s">
+        <v>2961</v>
+      </c>
+      <c r="AC15" s="16" t="s">
+        <v>2960</v>
+      </c>
+      <c r="AD15" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE15" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:36" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="34">
+        <v>356</v>
+      </c>
+      <c r="B16" s="34" t="s">
+        <v>1873</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D16" s="16">
+        <v>2020</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>2962</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>2963</v>
+      </c>
+      <c r="M16" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O16" s="16">
+        <v>2016</v>
+      </c>
+      <c r="S16" s="16" t="s">
+        <v>2964</v>
+      </c>
+      <c r="Z16" s="16" t="s">
+        <v>2961</v>
+      </c>
+      <c r="AC16" s="16" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD16" s="16" t="s">
+        <v>2967</v>
+      </c>
+      <c r="AE16" s="16" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="34">
+        <v>188</v>
+      </c>
+      <c r="B17" s="34" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D17" s="16">
+        <v>2008</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>2976</v>
+      </c>
+      <c r="F17" s="16" t="s">
+        <v>2928</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>2974</v>
+      </c>
+      <c r="M17" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O17" s="16">
+        <v>1997</v>
+      </c>
+      <c r="Q17" s="16">
+        <v>1600</v>
+      </c>
+      <c r="S17" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="V17" s="16">
+        <v>4</v>
+      </c>
+      <c r="X17" s="16">
+        <v>4</v>
+      </c>
+      <c r="Z17" s="16" t="s">
+        <v>2961</v>
+      </c>
+      <c r="AC17" s="16" t="s">
+        <v>2960</v>
+      </c>
+      <c r="AD17" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE17" s="16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="34">
+        <v>29</v>
+      </c>
+      <c r="B18" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1999</v>
+      </c>
+      <c r="F18" s="16" t="s">
+        <v>2977</v>
+      </c>
+      <c r="G18" s="16" t="s">
+        <v>2978</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>2979</v>
+      </c>
+      <c r="M18" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="AC18" s="16" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD18" s="16" t="s">
+        <v>2980</v>
+      </c>
+      <c r="AE18" s="16" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="34">
+        <v>29</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>183</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D19" s="16">
+        <v>1999</v>
+      </c>
+      <c r="F19" s="16" t="s">
+        <v>2977</v>
+      </c>
+      <c r="G19" s="16" t="s">
+        <v>2978</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>2979</v>
+      </c>
+      <c r="M19" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="AC19" s="16" t="s">
+        <v>2960</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="34">
+        <v>170</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>970</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D20" s="16">
+        <v>2020</v>
+      </c>
+      <c r="E20" s="16">
+        <v>2017</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>2949</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>2951</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>2912</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>2981</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O20" s="16">
+        <v>2017</v>
+      </c>
+      <c r="Q20" s="16">
+        <v>90000</v>
+      </c>
+      <c r="S20" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="Z20" s="16" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AB20" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC20" s="16" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD20" s="16" t="s">
+        <v>2934</v>
+      </c>
+      <c r="AE20" s="16" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="34">
+        <v>564</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>2826</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D21" s="16">
+        <v>2023</v>
+      </c>
+      <c r="E21" s="16">
+        <v>2020</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>2991</v>
+      </c>
+      <c r="G21" s="16" t="s">
+        <v>2951</v>
+      </c>
+      <c r="M21" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O21" s="16">
+        <v>2019</v>
+      </c>
+      <c r="R21" s="16" t="s">
+        <v>2987</v>
+      </c>
+      <c r="S21" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="T21" s="16">
+        <v>12</v>
+      </c>
+      <c r="U21" s="16">
+        <v>36</v>
+      </c>
+      <c r="V21" s="16">
+        <v>4</v>
+      </c>
+      <c r="X21" s="16">
+        <v>4</v>
+      </c>
+      <c r="Z21" s="16" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA21" s="16" t="s">
+        <v>2988</v>
+      </c>
+      <c r="AB21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC21" s="16" t="s">
+        <v>2989</v>
+      </c>
+      <c r="AE21" s="16" t="s">
+        <v>2990</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="34">
+        <v>562</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>2814</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D22" s="16">
+        <v>2023</v>
+      </c>
+      <c r="E22" s="16">
         <v>2021</v>
       </c>
-      <c r="F8" s="23" t="s">
-        <v>2929</v>
-      </c>
-      <c r="J8" s="23" t="s">
-        <v>2930</v>
-      </c>
-      <c r="L8" s="23" t="s">
-        <v>2900</v>
-      </c>
-      <c r="M8" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="N8" s="23">
-        <v>2009</v>
-      </c>
-      <c r="O8" s="23">
+      <c r="F22" s="16" t="s">
+        <v>2991</v>
+      </c>
+      <c r="G22" s="16" t="s">
+        <v>2992</v>
+      </c>
+      <c r="M22" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="T22" s="16">
+        <v>57</v>
+      </c>
+      <c r="Z22" s="16" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA22" s="16" t="s">
+        <v>2946</v>
+      </c>
+      <c r="AB22" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC22" s="16" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD22" s="16" t="s">
+        <v>2934</v>
+      </c>
+      <c r="AE22" s="16" t="s">
+        <v>2938</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="34">
+        <v>559</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>2795</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D23" s="16">
+        <v>2018</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>2995</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>2951</v>
+      </c>
+      <c r="M23" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O23" s="16">
+        <v>2014</v>
+      </c>
+      <c r="S23" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="Z23" s="16" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA23" s="16" t="s">
+        <v>2988</v>
+      </c>
+      <c r="AB23" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC23" s="16" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD23" s="16" t="s">
+        <v>2996</v>
+      </c>
+      <c r="AE23" s="16" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="34">
+        <v>545</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>2739</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D24" s="16">
+        <v>2024</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>2991</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>2951</v>
+      </c>
+      <c r="M24" s="16" t="s">
+        <v>2998</v>
+      </c>
+      <c r="P24" s="36" t="s">
+        <v>2999</v>
+      </c>
+      <c r="S24" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="T24" s="16">
+        <v>24</v>
+      </c>
+      <c r="Z24" s="16" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AC24" s="16" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD24" s="16" t="s">
+        <v>2953</v>
+      </c>
+      <c r="AE24" s="16" t="s">
+        <v>2935</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="34">
+        <v>541</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>2720</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D25" s="16">
+        <v>2023</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="34">
+        <v>537</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>2702</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D26" s="16">
+        <v>1994</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>3002</v>
+      </c>
+      <c r="M26" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O26" s="16">
+        <v>1988</v>
+      </c>
+      <c r="S26" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="AC26" s="16" t="s">
+        <v>3003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="34">
+        <v>534</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>2692</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D27" s="16">
+        <v>2022</v>
+      </c>
+      <c r="E27" s="16">
+        <v>2018</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>2949</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>2951</v>
+      </c>
+      <c r="M27" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="O27" s="16">
+        <v>2018</v>
+      </c>
+      <c r="P27" s="16" t="s">
+        <v>3005</v>
+      </c>
+      <c r="S27" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="T27" s="16">
+        <v>9</v>
+      </c>
+      <c r="U27" s="16">
+        <v>36</v>
+      </c>
+      <c r="V27" s="16">
+        <v>3</v>
+      </c>
+      <c r="X27" s="16">
+        <v>6</v>
+      </c>
+      <c r="Z27" s="16" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA27" s="16" t="s">
+        <v>2946</v>
+      </c>
+      <c r="AC27" s="16" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD27" s="16" t="s">
+        <v>2953</v>
+      </c>
+      <c r="AE27" s="16" t="s">
+        <v>2938</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="34">
+        <v>521</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>2635</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>3008</v>
+      </c>
+      <c r="D28" s="16">
+        <v>2020</v>
+      </c>
+      <c r="E28" s="16">
+        <v>2014</v>
+      </c>
+      <c r="F28" s="16" t="s">
+        <v>2995</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>2951</v>
+      </c>
+      <c r="K28" s="16" t="s">
+        <v>3009</v>
+      </c>
+      <c r="U28" s="16">
+        <v>135</v>
+      </c>
+      <c r="Z28" s="16" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA28" s="16" t="s">
+        <v>3010</v>
+      </c>
+      <c r="AB28" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC28" s="16" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD28" s="16" t="s">
+        <v>2953</v>
+      </c>
+      <c r="AE28" s="16" t="s">
+        <v>2954</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="34">
+        <v>498</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>2533</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D29" s="16">
+        <v>2017</v>
+      </c>
+      <c r="E29" s="16" t="s">
+        <v>3017</v>
+      </c>
+      <c r="F29" s="16" t="s">
+        <v>2995</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>2951</v>
+      </c>
+      <c r="J29" s="16" t="s">
+        <v>3016</v>
+      </c>
+      <c r="M29" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="P29" s="16">
         <v>8</v>
       </c>
-      <c r="P8" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q8" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="R8" s="23" t="s">
-        <v>2922</v>
-      </c>
-      <c r="S8" s="23">
-        <v>4</v>
-      </c>
-      <c r="U8" s="23" t="s">
-        <v>2932</v>
-      </c>
-      <c r="V8" s="23" t="s">
+      <c r="R29" s="16" t="s">
+        <v>3018</v>
+      </c>
+      <c r="S29" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="U29" s="16">
+        <v>27</v>
+      </c>
+      <c r="Z29" s="16" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA29" s="16" t="s">
+        <v>3019</v>
+      </c>
+      <c r="AC29" s="16" t="s">
         <v>2933</v>
       </c>
-      <c r="X8" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y8" s="23" t="s">
+    </row>
+    <row r="30" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="34">
+        <v>497</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>2527</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D30" s="16">
+        <v>2023</v>
+      </c>
+      <c r="E30" s="16">
+        <v>2020</v>
+      </c>
+      <c r="F30" s="16" t="s">
+        <v>3021</v>
+      </c>
+      <c r="K30" s="16" t="s">
+        <v>2959</v>
+      </c>
+      <c r="M30" s="16" t="s">
+        <v>2899</v>
+      </c>
+      <c r="P30" s="16">
+        <v>3</v>
+      </c>
+      <c r="S30" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="Z30" s="16" t="s">
+        <v>2931</v>
+      </c>
+      <c r="AA30" s="16" t="s">
+        <v>2946</v>
+      </c>
+      <c r="AB30" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="AC30" s="16" t="s">
+        <v>2933</v>
+      </c>
+      <c r="AD30" s="16" t="s">
         <v>2934</v>
       </c>
-      <c r="Z8" s="23" t="s">
-        <v>2935</v>
-      </c>
-      <c r="AA8" s="23" t="s">
-        <v>2936</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="16">
-        <v>452</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>2313</v>
-      </c>
-      <c r="C9" s="16" t="s">
-        <v>2899</v>
-      </c>
-      <c r="D9" s="16">
-        <v>2022</v>
-      </c>
-      <c r="E9" s="16">
-        <v>2015</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>2939</v>
-      </c>
-      <c r="J9" s="16" t="s">
-        <v>2942</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>2900</v>
-      </c>
-      <c r="N9" s="16">
-        <v>2012</v>
-      </c>
-      <c r="O9" s="16">
-        <v>3</v>
-      </c>
-      <c r="R9" s="16" t="s">
-        <v>2922</v>
-      </c>
-      <c r="T9" s="16">
-        <v>27</v>
-      </c>
-      <c r="U9" s="16" t="s">
-        <v>2932</v>
-      </c>
-      <c r="V9" s="16" t="s">
-        <v>2945</v>
-      </c>
-      <c r="W9" s="16">
-        <v>27</v>
-      </c>
-      <c r="X9" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y9" s="16" t="s">
-        <v>2934</v>
-      </c>
-      <c r="Z9" s="16" t="s">
-        <v>2935</v>
-      </c>
-      <c r="AA9" s="16" t="s">
-        <v>2940</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="16">
-        <v>396</v>
-      </c>
-      <c r="B10" s="16" t="s">
-        <v>2061</v>
-      </c>
-      <c r="C10" s="16" t="s">
-        <v>2899</v>
-      </c>
-      <c r="D10" s="16">
+      <c r="AE30" s="16" t="s">
+        <v>2938</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="34">
+        <v>491</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>2495</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>2898</v>
+      </c>
+      <c r="D31" s="16">
         <v>2004</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>2947</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>2907</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>2942</v>
-      </c>
-      <c r="L10" s="16" t="s">
-        <v>2900</v>
-      </c>
-      <c r="N10" s="16">
-        <v>1999</v>
-      </c>
-      <c r="R10" s="16" t="s">
-        <v>2922</v>
-      </c>
-      <c r="U10" s="16" t="s">
-        <v>2932</v>
-      </c>
-      <c r="V10" s="16" t="s">
-        <v>2948</v>
-      </c>
-      <c r="X10" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y10" s="16" t="s">
-        <v>2949</v>
-      </c>
-      <c r="Z10" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="AA10" s="16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="16">
-        <v>389</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>2028</v>
-      </c>
-      <c r="C11" s="16" t="s">
-        <v>2899</v>
-      </c>
-      <c r="D11" s="16">
-        <v>2019</v>
-      </c>
-      <c r="F11" s="16" t="s">
-        <v>2951</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>2953</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>2900</v>
-      </c>
-      <c r="N11" s="16">
-        <v>1995</v>
-      </c>
-      <c r="O11" s="16" t="s">
-        <v>2954</v>
-      </c>
-      <c r="U11" s="16" t="s">
-        <v>2932</v>
-      </c>
-      <c r="V11" s="16">
-        <v>18</v>
-      </c>
-      <c r="X11" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y11" s="16" t="s">
-        <v>2934</v>
-      </c>
-      <c r="Z11" s="16" t="s">
-        <v>2955</v>
-      </c>
-      <c r="AA11" s="16" t="s">
-        <v>2956</v>
-      </c>
-    </row>
-    <row r="12" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="16">
-        <v>389</v>
-      </c>
-      <c r="B12" s="16" t="s">
-        <v>2028</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>2919</v>
-      </c>
-      <c r="D12" s="16">
-        <v>2019</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>2951</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>2953</v>
-      </c>
-      <c r="L12" s="16" t="s">
-        <v>2900</v>
-      </c>
-      <c r="N12" s="16">
-        <v>1995</v>
-      </c>
-      <c r="O12" s="16" t="s">
-        <v>2954</v>
-      </c>
-      <c r="U12" s="16" t="s">
-        <v>2957</v>
-      </c>
-      <c r="Y12" s="16" t="s">
-        <v>2934</v>
-      </c>
-      <c r="Z12" s="16" t="s">
-        <v>2955</v>
-      </c>
-      <c r="AA12" s="16" t="s">
-        <v>2940</v>
-      </c>
-    </row>
-    <row r="13" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="18" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="19" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="20" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="21" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="22" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="23" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="24" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="E31" s="16" t="s">
+        <v>2994</v>
+      </c>
+      <c r="F31" s="16" t="s">
+        <v>2993</v>
+      </c>
+      <c r="G31" s="16" t="s">
+        <v>3023</v>
+      </c>
+      <c r="H31" s="16">
+        <v>-17.016667000000002</v>
+      </c>
+      <c r="I31" s="16">
+        <v>145.58333300000001</v>
+      </c>
+      <c r="J31" s="16" t="s">
+        <v>3024</v>
+      </c>
+      <c r="K31" s="16" t="s">
+        <v>2959</v>
+      </c>
+      <c r="L31" s="16" t="s">
+        <v>3025</v>
+      </c>
+      <c r="M31" s="16" t="s">
+        <v>2998</v>
+      </c>
+      <c r="N31" s="16" t="s">
+        <v>3026</v>
+      </c>
+      <c r="O31" s="16" t="s">
+        <v>2994</v>
+      </c>
+      <c r="P31" s="16" t="s">
+        <v>3005</v>
+      </c>
+      <c r="Q31" s="16" t="s">
+        <v>3027</v>
+      </c>
+      <c r="S31" s="16" t="s">
+        <v>2921</v>
+      </c>
+      <c r="Z31" s="16" t="s">
+        <v>2961</v>
+      </c>
+      <c r="AA31" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB31" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="AC31" s="16" t="s">
+        <v>2960</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="33" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="34" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -38350,8 +39757,10 @@
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="998" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="999" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <autoFilter ref="A1:AF1" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>